<commit_message>
Try algo lang muna for getting Student Number and saving
</commit_message>
<xml_diff>
--- a/Test-Data-for-Discrete-Hoho.xlsx
+++ b/Test-Data-for-Discrete-Hoho.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
@@ -647,8 +647,8 @@
   </sheetPr>
   <dimension ref="A1:H781"/>
   <sheetViews>
-    <sheetView topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B380" sqref="B380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20975,7 +20975,7 @@
   </sheetPr>
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EL MAO KA JEDD
</commit_message>
<xml_diff>
--- a/Test-Data-for-Discrete-Hoho.xlsx
+++ b/Test-Data-for-Discrete-Hoho.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5500" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5532" uniqueCount="120">
   <si>
     <t>P1</t>
   </si>
@@ -375,6 +375,12 @@
   <si>
     <t>Student_Number</t>
   </si>
+  <si>
+    <t>variable = male</t>
+  </si>
+  <si>
+    <t>variable = female</t>
+  </si>
 </sst>
 </file>
 
@@ -647,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:H781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20973,10 +20979,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20984,164 +20990,260 @@
     <col min="1" max="1" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>